<commit_message>
Zendodo to CNF conversion completed! - Added recursive cnf builder - Added FxE matrix creator
</commit_message>
<xml_diff>
--- a/data/zenodo_ivan/trade/CHE_trd_gas.xlsx
+++ b/data/zenodo_ivan/trade/CHE_trd_gas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/Downloads/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/trade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28141C4-A0A2-5647-B397-D956DFDB1D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338718E2-19F3-2D43-8CFC-06A8EADE7C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -266,16 +266,16 @@
     <t>Maximum historical import * 1.1</t>
   </si>
   <si>
-    <t>trd_coal</t>
-  </si>
-  <si>
     <t>output_efficiency</t>
   </si>
   <si>
-    <t>coal</t>
-  </si>
-  <si>
     <t>constant_fxe</t>
+  </si>
+  <si>
+    <t>trd_gas</t>
+  </si>
+  <si>
+    <t>gas</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -783,7 +783,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -800,7 +800,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -814,7 +814,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -828,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -842,7 +842,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -856,7 +856,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>28</v>
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>29</v>
@@ -896,7 +896,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>23</v>
@@ -922,7 +922,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>30</v>
@@ -936,7 +936,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>31</v>
@@ -950,16 +950,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" t="s">
         <v>78</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>80</v>
-      </c>
-      <c r="F16" t="s">
-        <v>79</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -973,7 +973,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
@@ -1005,7 +1005,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
@@ -1029,7 +1029,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>32</v>
@@ -1053,7 +1053,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
@@ -1077,7 +1077,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
@@ -1101,7 +1101,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -1125,7 +1125,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -1149,7 +1149,7 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -1173,7 +1173,7 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -1197,7 +1197,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
@@ -1221,7 +1221,7 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -1245,7 +1245,7 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
         <v>32</v>
@@ -1269,7 +1269,7 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
         <v>32</v>
@@ -1293,7 +1293,7 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
         <v>32</v>
@@ -1317,7 +1317,7 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
         <v>32</v>
@@ -1341,7 +1341,7 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
         <v>32</v>
@@ -1365,7 +1365,7 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
         <v>32</v>
@@ -1389,7 +1389,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
@@ -1413,7 +1413,7 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
@@ -1437,7 +1437,7 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
         <v>32</v>
@@ -1461,7 +1461,7 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C37" t="s">
         <v>32</v>
@@ -1485,7 +1485,7 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
         <v>32</v>
@@ -1509,7 +1509,7 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
         <v>32</v>
@@ -1533,7 +1533,7 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
         <v>32</v>
@@ -1557,7 +1557,7 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
         <v>32</v>
@@ -1581,7 +1581,7 @@
         <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
         <v>32</v>
@@ -1605,7 +1605,7 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
         <v>32</v>
@@ -1629,7 +1629,7 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
         <v>32</v>
@@ -1653,7 +1653,7 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
         <v>32</v>
@@ -1677,7 +1677,7 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
         <v>32</v>
@@ -1701,7 +1701,7 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
         <v>33</v>
@@ -1733,7 +1733,7 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
         <v>33</v>
@@ -1765,7 +1765,7 @@
         <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C49" t="s">
         <v>33</v>
@@ -1797,7 +1797,7 @@
         <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
         <v>33</v>
@@ -1829,7 +1829,7 @@
         <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C51" t="s">
         <v>33</v>
@@ -1861,7 +1861,7 @@
         <v>16</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
         <v>33</v>
@@ -1893,7 +1893,7 @@
         <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C53" t="s">
         <v>33</v>
@@ -1925,7 +1925,7 @@
         <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
         <v>33</v>
@@ -1957,7 +1957,7 @@
         <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
         <v>33</v>
@@ -1989,7 +1989,7 @@
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C56" t="s">
         <v>33</v>
@@ -2021,7 +2021,7 @@
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C57" t="s">
         <v>33</v>
@@ -2053,7 +2053,7 @@
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C58" t="s">
         <v>33</v>
@@ -2085,7 +2085,7 @@
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
         <v>33</v>
@@ -2117,7 +2117,7 @@
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
         <v>33</v>
@@ -2149,7 +2149,7 @@
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C61" t="s">
         <v>33</v>
@@ -2181,7 +2181,7 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C62" t="s">
         <v>33</v>
@@ -2213,7 +2213,7 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C63" t="s">
         <v>33</v>
@@ -2245,7 +2245,7 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
         <v>33</v>
@@ -2277,7 +2277,7 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C65" t="s">
         <v>33</v>
@@ -2309,7 +2309,7 @@
         <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
         <v>33</v>
@@ -2341,7 +2341,7 @@
         <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
         <v>33</v>
@@ -2373,7 +2373,7 @@
         <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
         <v>33</v>
@@ -2405,7 +2405,7 @@
         <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
         <v>33</v>
@@ -2437,7 +2437,7 @@
         <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C70" t="s">
         <v>33</v>
@@ -2469,7 +2469,7 @@
         <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C71" t="s">
         <v>33</v>
@@ -2501,7 +2501,7 @@
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C72" t="s">
         <v>33</v>
@@ -2533,7 +2533,7 @@
         <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C73" t="s">
         <v>33</v>
@@ -2565,7 +2565,7 @@
         <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C74" t="s">
         <v>33</v>
@@ -2597,7 +2597,7 @@
         <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C75" t="s">
         <v>33</v>
@@ -2629,7 +2629,7 @@
         <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C76" t="s">
         <v>33</v>
@@ -2661,7 +2661,7 @@
         <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C77" t="s">
         <v>34</v>
@@ -2693,7 +2693,7 @@
         <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
         <v>34</v>
@@ -2725,7 +2725,7 @@
         <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C79" t="s">
         <v>34</v>
@@ -2757,7 +2757,7 @@
         <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C80" t="s">
         <v>34</v>
@@ -2789,7 +2789,7 @@
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C81" t="s">
         <v>34</v>
@@ -2821,7 +2821,7 @@
         <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C82" t="s">
         <v>34</v>
@@ -2853,7 +2853,7 @@
         <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C83" t="s">
         <v>34</v>
@@ -2885,7 +2885,7 @@
         <v>16</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C84" t="s">
         <v>34</v>
@@ -2917,7 +2917,7 @@
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
         <v>34</v>
@@ -2949,7 +2949,7 @@
         <v>16</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C86" t="s">
         <v>34</v>
@@ -2981,7 +2981,7 @@
         <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C87" t="s">
         <v>34</v>
@@ -3013,7 +3013,7 @@
         <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C88" t="s">
         <v>34</v>
@@ -3045,7 +3045,7 @@
         <v>16</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C89" t="s">
         <v>34</v>
@@ -3077,7 +3077,7 @@
         <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C90" t="s">
         <v>34</v>
@@ -3109,7 +3109,7 @@
         <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C91" t="s">
         <v>34</v>
@@ -3141,7 +3141,7 @@
         <v>16</v>
       </c>
       <c r="B92" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C92" t="s">
         <v>34</v>
@@ -3173,7 +3173,7 @@
         <v>16</v>
       </c>
       <c r="B93" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C93" t="s">
         <v>34</v>
@@ -3205,7 +3205,7 @@
         <v>16</v>
       </c>
       <c r="B94" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C94" t="s">
         <v>34</v>
@@ -3237,7 +3237,7 @@
         <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C95" t="s">
         <v>34</v>
@@ -3269,7 +3269,7 @@
         <v>16</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C96" t="s">
         <v>34</v>
@@ -3301,7 +3301,7 @@
         <v>16</v>
       </c>
       <c r="B97" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C97" t="s">
         <v>34</v>
@@ -3333,7 +3333,7 @@
         <v>16</v>
       </c>
       <c r="B98" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C98" t="s">
         <v>34</v>
@@ -3365,7 +3365,7 @@
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C99" t="s">
         <v>34</v>
@@ -3397,7 +3397,7 @@
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C100" t="s">
         <v>34</v>
@@ -3429,7 +3429,7 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C101" t="s">
         <v>34</v>
@@ -3461,7 +3461,7 @@
         <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C102" t="s">
         <v>34</v>
@@ -3493,7 +3493,7 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C103" t="s">
         <v>34</v>
@@ -3525,7 +3525,7 @@
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C104" t="s">
         <v>34</v>
@@ -3557,7 +3557,7 @@
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C105" t="s">
         <v>34</v>
@@ -3589,7 +3589,7 @@
         <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C106" t="s">
         <v>34</v>

</xml_diff>